<commit_message>
PF de Sistemas Operativos
</commit_message>
<xml_diff>
--- a/Lab3_Archivos/datos_mediciones.xlsx
+++ b/Lab3_Archivos/datos_mediciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sole Cardozo\Documents\NDERAKORE\Lab3_Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sole Cardozo\Desktop\Laboratorios_SO_ElvisFretes\Lab3_Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B617518E-2276-4890-A9BD-38793A95282D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89B8042-BABC-4984-B52A-0AA0DAAEB46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,60 +20,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Sistema de Archivos</t>
   </si>
   <si>
-    <t>Tamaño de Archivo</t>
-  </si>
-  <si>
-    <t>Tiempo (segundos)</t>
-  </si>
-  <si>
-    <t>Unidad de Asignación</t>
-  </si>
-  <si>
-    <t>Notas</t>
+    <t>Tamaño del Archivo</t>
+  </si>
+  <si>
+    <t>Tiempo de Transferencia</t>
+  </si>
+  <si>
+    <t>exFAT</t>
   </si>
   <si>
     <t>NTFS</t>
   </si>
   <si>
-    <t>exFAT</t>
-  </si>
-  <si>
-    <t>Pequeño (KB)</t>
-  </si>
-  <si>
-    <t>Mediano (MB)</t>
-  </si>
-  <si>
-    <t>Grande (GB)</t>
-  </si>
-  <si>
-    <t>4096 bytes</t>
-  </si>
-  <si>
-    <t>128 KB</t>
-  </si>
-  <si>
-    <t>Archivo pequeño, sin diferencias notables</t>
-  </si>
-  <si>
-    <t>Tarda más que exFAT con este tamaño</t>
-  </si>
-  <si>
-    <t>Mismo tiempo que exFAT, limitado por USB</t>
-  </si>
-  <si>
-    <t>Igual velocidad que NTFS para archivos pequeños</t>
-  </si>
-  <si>
-    <t>Más rápido que NTFS con este tamaño</t>
-  </si>
-  <si>
-    <t>Mismo tiempo que NTFS, limitado por USB</t>
+    <t>1 seg</t>
+  </si>
+  <si>
+    <t>10 seg</t>
+  </si>
+  <si>
+    <t>11 min</t>
+  </si>
+  <si>
+    <t>2 min 15 seg</t>
+  </si>
+  <si>
+    <t>500 KB</t>
+  </si>
+  <si>
+    <t>500 MB</t>
+  </si>
+  <si>
+    <t>1 GB</t>
   </si>
 </sst>
 </file>
@@ -132,11 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,20 +458,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,113 +481,71 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C3">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>3900</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>3900</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>